<commit_message>
ready for document analyzer
</commit_message>
<xml_diff>
--- a/evl_streaming_src/results/Results.xlsx
+++ b/evl_streaming_src/results/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.6004999999999999</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>11192.76840257645</v>
+        <v>28.96503901481628</v>
       </c>
     </row>
     <row r="3">
@@ -504,7 +504,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.6004999999999999</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>36339.18366360664</v>
+        <v>2.488220691680908</v>
       </c>
     </row>
     <row r="4">
@@ -532,7 +532,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.1975</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -541,7 +541,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>30692.68313479424</v>
+        <v>4.691967964172363</v>
       </c>
     </row>
     <row r="5">
@@ -555,12 +555,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>scargc_JITC_naive_bayes_UNSW</t>
+          <t>scargc_JITC_adaboost_UNSW</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.9997594250513346</t>
+          <t>0.6004999999999999</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>699.9430840015411</v>
+        <v>31.99111533164978</v>
       </c>
     </row>
     <row r="6">
@@ -583,21 +583,49 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>scargc_JITC_naive_bayes_UNSW</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.1975</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Only one class found</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1.328789710998535</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>JITC</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>scargc_JITC_logistic_regression_UNSW</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.9999563449691992</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.48575</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Only one class found</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>3093.229716300964</v>
+      <c r="F7" t="n">
+        <v>6.465306520462036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>